<commit_message>
Added several features, see log for detail
Improved automated standard_values, improved object-oriented programming, started adding commercial sector buildings
</commit_message>
<xml_diff>
--- a/upscaling_scenario_tool/test_scenario.xlsx
+++ b/upscaling_scenario_tool/test_scenario.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="171">
   <si>
     <t>start date</t>
   </si>
@@ -98,22 +98,19 @@
     <t>central_swhp_elec_bus</t>
   </si>
   <si>
-    <t>sdb004_electricity_bus</t>
-  </si>
-  <si>
-    <t>sdb004_heat_bus</t>
-  </si>
-  <si>
-    <t>sdb004_hp_elec_bus</t>
-  </si>
-  <si>
-    <t>sdb004_pv_bus</t>
-  </si>
-  <si>
-    <t>sdb004_gas_bus</t>
-  </si>
-  <si>
-    <t>upscaling</t>
+    <t>DENW05AL10000uaC_electricity_bus</t>
+  </si>
+  <si>
+    <t>DENW05AL10000uaC_heat_bus</t>
+  </si>
+  <si>
+    <t>DENW05AL10000uaC_hp_elec_bus</t>
+  </si>
+  <si>
+    <t>DENW05AL10000uaC_pv_bus</t>
+  </si>
+  <si>
+    <t>DENW05AL10000uaC_gas_bus</t>
   </si>
   <si>
     <t>automatically created</t>
@@ -146,16 +143,16 @@
     <t>wind class [HEAT SLP ONLY]</t>
   </si>
   <si>
-    <t>sdb004_electricity_demand</t>
-  </si>
-  <si>
-    <t>sdb004_heat_demand</t>
-  </si>
-  <si>
-    <t>h0</t>
-  </si>
-  <si>
-    <t>efh</t>
+    <t>DENW05AL10000uaC_electricity_demand</t>
+  </si>
+  <si>
+    <t>DENW05AL10000uaC_heat_demand</t>
+  </si>
+  <si>
+    <t>g0</t>
+  </si>
+  <si>
+    <t>GKO</t>
   </si>
   <si>
     <t>x</t>
@@ -230,10 +227,19 @@
     <t>Capacity per Area (kW/m2)</t>
   </si>
   <si>
-    <t>sdb004_1_pv_source</t>
-  </si>
-  <si>
-    <t>sdb004_2_pv_source</t>
+    <t>Unnamed: 17</t>
+  </si>
+  <si>
+    <t>Unnamed: 18</t>
+  </si>
+  <si>
+    <t>Unnamed: 19</t>
+  </si>
+  <si>
+    <t>DENW05AL10000uaC_1_pv_source</t>
+  </si>
+  <si>
+    <t>DENW05AL10000uaC_2_pv_source</t>
   </si>
   <si>
     <t>fixed photovoltaic source</t>
@@ -332,7 +338,7 @@
     <t>biogas_chp_transformer</t>
   </si>
   <si>
-    <t>sdb004_gasheating_transformer</t>
+    <t>DENW05AL10000uaC_gasheating_transformer</t>
   </si>
   <si>
     <t>automatically_created</t>
@@ -413,10 +419,7 @@
     <t>central_swhp_transformer</t>
   </si>
   <si>
-    <t>sdb004_gchp_transformer</t>
-  </si>
-  <si>
-    <t>sdb004_ashp_transformer</t>
+    <t>DENW05AL10000uaC_gchp_transformer</t>
   </si>
   <si>
     <t>HeatPump</t>
@@ -434,9 +437,6 @@
     <t>Ground</t>
   </si>
   <si>
-    <t>Air</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -503,12 +503,6 @@
     <t>variable output costs</t>
   </si>
   <si>
-    <t>sdb004_battery_storage</t>
-  </si>
-  <si>
-    <t>Generic</t>
-  </si>
-  <si>
     <t>diameter /m</t>
   </si>
   <si>
@@ -524,25 +518,31 @@
     <t>(un)directed</t>
   </si>
   <si>
+    <t>link_type</t>
+  </si>
+  <si>
     <t>district_heat_link</t>
   </si>
   <si>
-    <t>sdb004_gchp_building_link</t>
-  </si>
-  <si>
-    <t>sdb004_district_heat_link</t>
-  </si>
-  <si>
-    <t>sdb004pv_sdb004_electricity_link</t>
-  </si>
-  <si>
-    <t>sdb004pv_district_electricity_link</t>
-  </si>
-  <si>
-    <t>sdb004district_electricity_link</t>
+    <t>DENW05AL10000uaC_gchp_building_link</t>
+  </si>
+  <si>
+    <t>DENW05AL10000uaC_district_heat_link</t>
+  </si>
+  <si>
+    <t>DENW05AL10000uaCpv_DENW05AL10000uaC_electricity_link</t>
+  </si>
+  <si>
+    <t>DENW05AL10000uaCpv_district_electricity_link</t>
+  </si>
+  <si>
+    <t>DENW05AL10000uaCdistrict_electricity_link</t>
   </si>
   <si>
     <t>directed</t>
+  </si>
+  <si>
+    <t>building_hp_elec_link</t>
   </si>
 </sst>
 </file>
@@ -941,84 +941,84 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="W1" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -1075,21 +1075,21 @@
         <v>0</v>
       </c>
       <c r="W2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -1146,21 +1146,21 @@
         <v>0</v>
       </c>
       <c r="W3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
@@ -1169,13 +1169,13 @@
         <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H4">
         <v>0.85</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J4">
         <v>200</v>
@@ -1235,88 +1235,88 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1326,7 +1326,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1337,117 +1337,117 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="X1" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:33">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F2" t="s">
         <v>21</v>
@@ -1456,13 +1456,13 @@
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1504,13 +1504,13 @@
         <v>0</v>
       </c>
       <c r="X2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Y2">
         <v>60</v>
       </c>
       <c r="Z2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA2">
         <v>0.5</v>
@@ -1536,19 +1536,19 @@
     </row>
     <row r="3" spans="1:33">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -1557,13 +1557,13 @@
         <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I3">
         <v>0.95</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K3">
         <v>10</v>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N3">
         <v>0.1</v>
@@ -1605,19 +1605,19 @@
         <v>0</v>
       </c>
       <c r="X3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Y3">
         <v>60</v>
       </c>
       <c r="Z3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA3">
         <v>0.55</v>
       </c>
       <c r="AB3">
-        <v>800</v>
+        <v>100</v>
       </c>
       <c r="AC3">
         <v>100</v>
@@ -1633,107 +1633,6 @@
       </c>
       <c r="AG3">
         <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33">
-      <c r="A4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>103</v>
-      </c>
-      <c r="I4">
-        <v>0.95</v>
-      </c>
-      <c r="J4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4">
-        <v>10</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4">
-        <v>0.1</v>
-      </c>
-      <c r="O4">
-        <v>0.1</v>
-      </c>
-      <c r="P4">
-        <v>0.1</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>100</v>
-      </c>
-      <c r="S4">
-        <v>1000</v>
-      </c>
-      <c r="T4">
-        <v>110</v>
-      </c>
-      <c r="U4">
-        <v>0.1</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y4">
-        <v>40</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA4">
-        <v>0.4</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>3</v>
-      </c>
-      <c r="AG4">
-        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -1754,70 +1653,70 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>135</v>
@@ -1842,7 +1741,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1853,7 +1752,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
@@ -1880,10 +1779,10 @@
         <v>146</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>147</v>
@@ -1916,84 +1815,10 @@
         <v>156</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>50</v>
-      </c>
-      <c r="H2">
-        <v>1000</v>
-      </c>
-      <c r="I2">
-        <v>70</v>
-      </c>
-      <c r="J2">
-        <v>0.1</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0.17</v>
-      </c>
-      <c r="N2">
-        <v>0.17</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>0.98</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0.1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0.1</v>
-      </c>
-      <c r="X2">
-        <v>0.1</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2014,7 +1839,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
@@ -2041,10 +1866,10 @@
         <v>146</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>147</v>
@@ -2074,22 +1899,22 @@
         <v>156</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2099,68 +1924,71 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
         <v>163</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>164</v>
-      </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2172,45 +2000,48 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>9999999</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
         <v>170</v>
       </c>
-      <c r="G2">
-        <v>0.85</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0.1</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>99999999</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>0.1</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2222,7 +2053,7 @@
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2254,13 +2085,16 @@
       <c r="P3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2272,7 +2106,7 @@
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -2304,13 +2138,16 @@
       <c r="P4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2322,7 +2159,7 @@
         <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -2354,13 +2191,16 @@
       <c r="P5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2372,7 +2212,7 @@
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -2404,13 +2244,16 @@
       <c r="P6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2422,13 +2265,13 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -2453,6 +2296,9 @@
       </c>
       <c r="P7">
         <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2552,7 +2398,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2581,7 +2427,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2610,7 +2456,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2639,7 +2485,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2668,7 +2514,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2697,7 +2543,7 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2726,7 +2572,7 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2755,7 +2601,7 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2784,7 +2630,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2813,7 +2659,7 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2842,7 +2688,7 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2871,7 +2717,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2913,39 +2759,39 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -2960,27 +2806,27 @@
         <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2">
-        <v>4000</v>
+        <v>11267.704005228</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -2995,22 +2841,22 @@
         <v>23</v>
       </c>
       <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
         <v>41</v>
       </c>
-      <c r="G3" t="s">
-        <v>42</v>
-      </c>
       <c r="H3">
-        <v>44460</v>
+        <v>30320.3671413408</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3020,98 +2866,107 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:26">
+      <c r="AB1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3120,7 +2975,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
         <v>25</v>
@@ -3138,7 +2993,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>7.03</v>
+        <v>0.350892</v>
       </c>
       <c r="L2">
         <v>90</v>
@@ -3153,22 +3008,22 @@
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Q2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="R2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="S2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="T2">
-        <v>238</v>
+        <v>-115.670163645254</v>
       </c>
       <c r="U2">
-        <v>29</v>
+        <v>40.6717119369133</v>
       </c>
       <c r="V2">
         <v>0.18</v>
@@ -3186,12 +3041,12 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3200,7 +3055,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>
@@ -3218,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>4.56</v>
+        <v>0.350892</v>
       </c>
       <c r="L3">
         <v>90</v>
@@ -3233,22 +3088,22 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Q3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="R3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="S3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="T3">
-        <v>59</v>
+        <v>-115.670163645254</v>
       </c>
       <c r="U3">
-        <v>29</v>
+        <v>40.6717119369133</v>
       </c>
       <c r="V3">
         <v>0.18</v>
@@ -3284,94 +3139,94 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="Q1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3392,85 +3247,85 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="Q1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3491,46 +3346,46 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -3551,52 +3406,52 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -3617,46 +3472,46 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>